<commit_message>
adds missing unit to trap metadata file
</commit_message>
<xml_diff>
--- a/data-raw/metadata/camp_trap_metadata.xlsx
+++ b/data-raw/metadata/camp_trap_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-knights-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3691F8E-CB2B-6A45-83BF-8A11446F458C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2032797-219F-E544-A4C6-57F085B356C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="68640" yWindow="-12120" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="170">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -542,6 +542,9 @@
   <si>
     <t>2022-05-18 02:30:56</t>
   </si>
+  <si>
+    <t>see unit column</t>
+  </si>
 </sst>
 </file>
 
@@ -651,11 +654,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -874,7 +877,7 @@
   <dimension ref="A1:Z1010"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1124,10 +1127,10 @@
         <v>30</v>
       </c>
       <c r="K6" s="2"/>
-      <c r="L6" s="20" t="s">
+      <c r="L6" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="M6" s="20" t="s">
+      <c r="M6" s="18" t="s">
         <v>168</v>
       </c>
       <c r="N6" s="1"/>
@@ -1168,10 +1171,10 @@
         <v>30</v>
       </c>
       <c r="K7" s="2"/>
-      <c r="L7" s="20" t="s">
+      <c r="L7" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="M7" s="20" t="s">
+      <c r="M7" s="18" t="s">
         <v>168</v>
       </c>
       <c r="N7" s="1"/>
@@ -1761,7 +1764,9 @@
       <c r="F21" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G21" s="3"/>
+      <c r="G21" s="3" t="s">
+        <v>169</v>
+      </c>
       <c r="H21" s="3" t="s">
         <v>46</v>
       </c>
@@ -2439,7 +2444,7 @@
       <c r="Z46" s="1"/>
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="18"/>
+      <c r="A47" s="19"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="2"/>
@@ -2467,7 +2472,7 @@
       <c r="Z47" s="1"/>
     </row>
     <row r="48" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="19"/>
+      <c r="A48" s="20"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="2"/>
@@ -2495,7 +2500,7 @@
       <c r="Z48" s="1"/>
     </row>
     <row r="49" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="18"/>
+      <c r="A49" s="19"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="2"/>
@@ -2523,7 +2528,7 @@
       <c r="Z49" s="1"/>
     </row>
     <row r="50" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="19"/>
+      <c r="A50" s="20"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="2"/>

</xml_diff>